<commit_message>
update company and contract and action code and module
</commit_message>
<xml_diff>
--- a/database/seeders/excel/module.xlsx
+++ b/database/seeders/excel/module.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\niise_helpdesk\be\database\seeders\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadnajmibinsidek/Developer/niise-helpdesk/backend/database/seeders/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662C70A7-92D5-FD4F-B022-E0364D60FF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="23040" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="117">
   <si>
     <t>dashboard</t>
   </si>
@@ -47,7 +49,7 @@
     <t>Controls user access, system-level settings, and configurations for managing the application.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;g transform='translate(-2.1,-2.2) scale(1.18)'&gt;&lt;path opacity='0.4' d='M16.19 2H7.81C4.17 2 2 4.17 2 7.81V16.18C2 19.83 4.17 22 7.81 22H16.18C19.82 22 21.99 19.83 21.99 16.19V7.81C22 4.17 19.83 2 16.19 2Z' fill='currentColor'&gt;&lt;/path&gt;
+    <t>&lt;g transform='translate(-2.1,-2.2) scale(1.18)'&gt;&lt;path opacity='0.4' d='M16.19 2H7.81C4.17 2 2 4.17 2 7.81V16.18C2 19.83 4.17 22 7.81 22H16.18C19.82 22 21.99 19.83 21.99 16.19V7.81C22 4.17 19.83 2 16.19 2Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path d='M15.5801 19.2501C15.1701 19.2501 14.8301 18.9101 14.8301 18.5001V14.6001C14.8301 14.1901 15.1701 13.8501 15.5801 13.8501C15.9901 13.8501 16.3301 14.1901 16.3301 14.6001V18.5001C16.3301 18.9101 15.9901 19.2501 15.5801 19.2501Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path d='M15.5801 8.2C15.1701 8.2 14.8301 7.86 14.8301 7.45V5.5C14.8301 5.09 15.1701 4.75 15.5801 4.75C15.9901 4.75 16.3301 5.09 16.3301 5.5V7.45C16.3301 7.86 15.9901 8.2 15.5801 8.2Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path d='M8.41992 19.2498C8.00992 19.2498 7.66992 18.9098 7.66992 18.4998V16.5498C7.66992 16.1398 8.00992 15.7998 8.41992 15.7998C8.82992 15.7998 9.16992 16.1398 9.16992 16.5498V18.4998C9.16992 18.9098 8.83992 19.2498 8.41992 19.2498Z' fill='currentColor'&gt;&lt;/path&gt;
@@ -75,9 +77,6 @@
     <t>individuals</t>
   </si>
   <si>
-    <t>Pengurusan Individu</t>
-  </si>
-  <si>
     <t>Individual Management</t>
   </si>
   <si>
@@ -321,7 +320,7 @@
     <t>Tracks and manages incidents, tickets, or issues reported by users or detected by the system.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;g transform='translate(-1.2,-1.2) scale(1.10)'&gt;
+    <t>&lt;g transform='translate(-1.2,-1.2) scale(1.10)'&gt;
                                 &lt;path opacity='0.5' d='M4 16V21.25H20V16C20 11.5817 16.4183 8 12 8C7.58172 8 4 11.5817 4 16Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path d='M12.75 2C12.75 1.58579 12.4142 1.25 12 1.25C11.5858 1.25 11.25 1.58579 11.25 2V5C11.25 5.41421 11.5858 5.75 12 5.75C12.4142 5.75 12.75 5.41421 12.75 5V2Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path d='M21.5303 5.46967C21.8232 5.76256 21.8232 6.23744 21.5303 6.53033L20.0303 8.03033C19.7374 8.32322 19.2626 8.32322 18.9697 8.03033C18.6768 7.73744 18.6768 7.26256 18.9697 6.96967L20.4697 5.46967C20.7626 5.17678 21.2374 5.17678 21.5303 5.46967Z' fill='currentColor'&gt;&lt;/path&gt;
@@ -347,7 +346,7 @@
     <t>Logs of user activities, changes, and system events for monitoring and security.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;g transform='translate(-1.2,-2.2) scale(1.18)'&gt;
+    <t>&lt;g transform='translate(-1.2,-2.2) scale(1.18)'&gt;
                                 &lt;path opacity='0.5' d='M12 20.0283V18H8L8 20.0283C8 20.3054 8 20.444 8.09485 20.5C8.18971 20.556 8.31943 20.494 8.57888 20.3701L9.82112 19.7766C9.9089 19.7347 9.95279 19.7138 10 19.7138C10.0472 19.7138 10.0911 19.7347 10.1789 19.7767L11.4211 20.3701C11.6806 20.494 11.8103 20.556 11.9051 20.5C12 20.444 12 20.3054 12 20.0283Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path d='M8 18H7.42598C6.34236 18 5.96352 18.0057 5.67321 18.0681C5.15982 18.1785 4.71351 18.4151 4.38811 18.7347C4.27837 18.8425 4.22351 18.8964 4.09696 19.2397C3.97041 19.5831 3.99045 19.7288 4.03053 20.02C4.03761 20.0714 4.04522 20.1216 4.05343 20.1706C4.16271 20.8228 4.36259 21.1682 4.66916 21.4142C4.97573 21.6602 5.40616 21.8206 6.21896 21.9083C7.05566 21.9986 8.1646 22 9.75461 22H14.1854C15.7754 22 16.8844 21.9986 17.7211 21.9083C18.5339 21.8206 18.9643 21.6602 19.2709 21.4142C19.5774 21.1682 19.7773 20.8228 19.8866 20.1706C19.9784 19.6228 19.9965 18.9296 20 18H12V20.0283C12 20.3054 12 20.444 11.9051 20.5C11.8103 20.556 11.6806 20.494 11.4211 20.3701L10.1789 19.7767C10.0911 19.7347 10.0472 19.7138 10 19.7138C9.95279 19.7138 9.9089 19.7347 9.82112 19.7766L8.57888 20.3701C8.31943 20.494 8.18971 20.556 8.09485 20.5C8 20.444 8 20.3054 8 20.0283V18Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path opacity='0.5' d='M4.72718 2.73332C5.03258 2.42535 5.46135 2.22456 6.27103 2.11478C7.10452 2.00177 8.2092 2 9.7931 2H14.2069C15.7908 2 16.8955 2.00177 17.729 2.11478C18.5387 2.22456 18.9674 2.42535 19.2728 2.73332C19.5782 3.0413 19.7773 3.47368 19.8862 4.2902C19.9982 5.13073 20 6.24474 20 7.84202L20 18H7.42598C6.34236 18 5.96352 18.0057 5.67321 18.0681C5.15982 18.1785 4.71351 18.4151 4.38811 18.7347C4.27837 18.8425 4.22351 18.8964 4.09696 19.2397C4.02435 19.4367 4 19.5687 4 19.7003V7.84202C4 6.24474 4.00176 5.13073 4.11382 4.2902C4.22268 3.47368 4.42179 3.0413 4.72718 2.73332Z' fill='currentColor'&gt;&lt;/path&gt;
@@ -371,7 +370,7 @@
     <t>Generates and displays data summaries, charts, and analytics on system usage and performance.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;g transform='translate(-2.2,-2.1) scale(1.18)'&gt;
+    <t>&lt;g transform='translate(-2.2,-2.1) scale(1.18)'&gt;
                                 &lt;path opacity='0.5' d='M21 15.9983V9.99826C21 7.16983 21 5.75562 20.1213 4.87694C19.3529 4.10856 18.175 4.01211 16 4H8C5.82497 4.01211 4.64706 4.10856 3.87868 4.87694C3 5.75562 3 7.16983 3 9.99826V15.9983C3 18.8267 3 20.2409 3.87868 21.1196C4.75736 21.9983 6.17157 21.9983 9 21.9983H15C17.8284 21.9983 19.2426 21.9983 20.1213 21.1196C21 20.2409 21 18.8267 21 15.9983Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path d='M8 3.5C8 2.67157 8.67157 2 9.5 2H14.5C15.3284 2 16 2.67157 16 3.5V4.5C16 5.32843 15.3284 6 14.5 6H9.5C8.67157 6 8 5.32843 8 4.5V3.5Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path fill-rule='evenodd' clip-rule='evenodd' d='M6.25 10.5C6.25 10.0858 6.58579 9.75 7 9.75H17C17.4142 9.75 17.75 10.0858 17.75 10.5C17.75 10.9142 17.4142 11.25 17 11.25H7C6.58579 11.25 6.25 10.9142 6.25 10.5ZM7.25 14C7.25 13.5858 7.58579 13.25 8 13.25H16C16.4142 13.25 16.75 13.5858 16.75 14C16.75 14.4142 16.4142 14.75 16 14.75H8C7.58579 14.75 7.25 14.4142 7.25 14ZM8.25 17.5C8.25 17.0858 8.58579 16.75 9 16.75H15C15.4142 16.75 15.75 17.0858 15.75 17.5C15.75 17.9142 15.4142 18.25 15 18.25H9C8.58579 18.25 8.25 17.9142 8.25 17.5Z' fill='currentColor'&gt;&lt;/path&gt;
@@ -390,20 +389,23 @@
     <t>A collection of helpful articles, FAQs, and documentation to guide users and reduce support load.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;g id='SVGRepo_iconCarrier' transform='translate(-2.2,-2.1) scale(1.18)'&gt;
+    <t>&lt;g id='SVGRepo_iconCarrier' transform='translate(-2.2,-2.1) scale(1.18)'&gt;
                                 &lt;path opacity='0.5' d='M16.5 3H7.5C6.39543 3 5.5 3.52941 5 5.11765L2.15737 14.9263C2.20285 14.7794 2.26148 14.6491 2.33706 14.5294C2.48298 14.2982 2.67048 14.0996 2.88886 13.9451C3.39331 13.5882 4.09554 13.5882 5.5 13.5882H18.5C19.9045 13.5882 20.6067 13.5882 21.1111 13.9451C21.3295 14.0996 21.517 14.2982 21.6629 14.5294C21.7435 14.6571 21.8049 14.7968 21.8515 14.9557L19 5.11765C18.5 3.52941 17.6046 3 16.5 3Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;path fill-rule='evenodd' clip-rule='evenodd' d='M5.5 13.5879H18.5C19.9045 13.5879 20.6067 13.5879 21.1111 13.9448C21.3295 14.0993 21.517 14.2978 21.6629 14.529C21.7435 14.6567 21.8049 14.7965 21.8515 14.9554C22 15.4611 22 16.1618 22 17.2929C22 18.7799 22 19.5244 21.6629 20.0585C21.517 20.2897 21.3295 20.4883 21.1111 20.6428C20.6067 20.9997 19.9045 20.9997 18.5 20.9997H5.5C4.09554 20.9997 3.39331 20.9997 2.88886 20.6428C2.67048 20.4883 2.48298 20.2897 2.33706 20.0585C2 19.5244 2 18.7809 2 17.2938C2 16.1949 2 15.502 2.136 14.9997C2.14278 14.9746 2.1499 14.95 2.15737 14.9259C2.20285 14.7791 2.26148 14.6488 2.33706 14.529C2.48298 14.2978 2.67048 14.0993 2.88886 13.9448C3.39331 13.5879 4.09554 13.5879 5.5 13.5879ZM19 16.25C19.4142 16.25 19.75 16.5858 19.75 17V18C19.75 18.4142 19.4142 18.75 19 18.75C18.5858 18.75 18.25 18.4142 18.25 18V17C18.25 16.5858 18.5858 16.25 19 16.25ZM17.25 17C17.25 16.5858 16.9142 16.25 16.5 16.25C16.0858 16.25 15.75 16.5858 15.75 17V18C15.75 18.4142 16.0858 18.75 16.5 18.75C16.9142 18.75 17.25 18.4142 17.25 18V17ZM14 16.25C14.4142 16.25 14.75 16.5858 14.75 17V18C14.75 18.4142 14.4142 18.75 14 18.75C13.5858 18.75 13.25 18.4142 13.25 18V17C13.25 16.5858 13.5858 16.25 14 16.25ZM12.25 17C12.25 16.5858 11.9142 16.25 11.5 16.25C11.0858 16.25 10.75 16.5858 10.75 17V18C10.75 18.4142 11.0858 18.75 11.5 18.75C11.9142 18.75 12.25 18.4142 12.25 18V17Z' fill='currentColor'&gt;&lt;/path&gt;
                                 &lt;/g&gt;</t>
   </si>
   <si>
     <t>knowledge-base</t>
+  </si>
+  <si>
+    <t>Pengurusan Pengguna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,7 +423,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -434,6 +442,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -442,10 +458,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -725,28 +741,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C12"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.75" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="43" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="81.875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="81.83203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -804,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -836,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -844,13 +863,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -859,165 +878,165 @@
         <v>15</v>
       </c>
       <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>19</v>
-      </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>24</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>29</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
       </c>
       <c r="G7">
         <v>5</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>34</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1035,255 +1054,255 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
         <v>47</v>
       </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>51</v>
       </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" t="s">
         <v>52</v>
       </c>
-      <c r="H11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>53</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>56</v>
       </c>
-      <c r="E12" t="s">
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" t="s">
         <v>57</v>
       </c>
-      <c r="H12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>58</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>59</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
         <v>60</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>61</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>62</v>
-      </c>
-      <c r="F13" t="s">
-        <v>63</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>66</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>67</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" t="s">
         <v>68</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>69</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
         <v>70</v>
       </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>71</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>72</v>
-      </c>
-      <c r="E15" t="s">
-        <v>73</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J15">
         <v>1</v>
@@ -1301,281 +1320,281 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
         <v>75</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>76</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>77</v>
-      </c>
-      <c r="F16" t="s">
-        <v>78</v>
       </c>
       <c r="G16">
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J16">
         <v>1</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
         <v>79</v>
       </c>
-      <c r="B17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>80</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>81</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I17" t="s">
         <v>82</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="s">
-        <v>79</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>83</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
         <v>84</v>
       </c>
-      <c r="B18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>85</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>87</v>
       </c>
       <c r="G18">
         <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I18" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>88</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" t="s">
         <v>89</v>
       </c>
-      <c r="B19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>90</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>91</v>
-      </c>
-      <c r="E19" t="s">
-        <v>92</v>
       </c>
       <c r="G19">
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>93</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
         <v>94</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>95</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>96</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>97</v>
-      </c>
-      <c r="F20" t="s">
-        <v>98</v>
       </c>
       <c r="G20">
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I20" t="s">
+        <v>98</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>99</v>
       </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
         <v>100</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>101</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>102</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>103</v>
-      </c>
-      <c r="F21" t="s">
-        <v>104</v>
       </c>
       <c r="G21">
         <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>105</v>
       </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
         <v>106</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>107</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>108</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>109</v>
-      </c>
-      <c r="F22" t="s">
-        <v>110</v>
       </c>
       <c r="G22">
         <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I22" t="s">
+        <v>110</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>111</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
         <v>112</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" t="s">
         <v>113</v>
       </c>
-      <c r="D23" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>114</v>
-      </c>
-      <c r="F23" t="s">
-        <v>115</v>
       </c>
       <c r="G23">
         <v>6</v>
       </c>
       <c r="H23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -1594,6 +1613,7 @@
       </c>
     </row>
   </sheetData>
-  <pageSetup r:id="rId1" orientation="portrait"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update backend middleware and api for admin and access viewlog
</commit_message>
<xml_diff>
--- a/database/seeders/excel/module.xlsx
+++ b/database/seeders/excel/module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadnajmibinsidek/Developer/niise-helpdesk/backend/database/seeders/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754CAA33-532B-0442-AFEA-16A820911129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6006B7F-57A9-8E4E-89EE-CE549D41DC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="116">
   <si>
     <t>dashboard</t>
   </si>
@@ -362,9 +362,6 @@
     <t>incident_details</t>
   </si>
   <si>
-    <t>API Logs</t>
-  </si>
-  <si>
     <t>queue</t>
   </si>
   <si>
@@ -384,6 +381,21 @@
   </si>
   <si>
     <t>Pengurusan Individu</t>
+  </si>
+  <si>
+    <t>Laporan Khas</t>
+  </si>
+  <si>
+    <t>Reports Special</t>
+  </si>
+  <si>
+    <t>Generates special report and displays data summaries on system usage and performance.</t>
+  </si>
+  <si>
+    <t>special_reports</t>
+  </si>
+  <si>
+    <t>Backend Logs</t>
   </si>
 </sst>
 </file>
@@ -733,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -821,7 +833,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -1207,7 +1219,7 @@
         <v>98</v>
       </c>
       <c r="G23">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1235,10 +1247,10 @@
         <v>100</v>
       </c>
       <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" t="s">
         <v>107</v>
-      </c>
-      <c r="D25" t="s">
-        <v>108</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1246,16 +1258,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
         <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -1263,19 +1275,39 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
         <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G27">
         <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>